<commit_message>
feat/ adding additional courses I've played
</commit_message>
<xml_diff>
--- a/app/data/Course_Data.xlsx
+++ b/app/data/Course_Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="23">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -71,6 +71,24 @@
   </si>
   <si>
     <t xml:space="preserve">Berhampore Golf Course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chamberlain Park Golf Course </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manawatu Golf Club </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palmerston North Golf Club </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-40.35269116882644</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waimairi Beach Golf Course </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-43.48113500900837</t>
   </si>
 </sst>
 </file>
@@ -155,7 +173,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -165,11 +183,23 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -361,15 +391,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:H154"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N86" activeCellId="0" sqref="N86"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="H56" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
+      <selection pane="bottomRight" activeCell="J67" activeCellId="0" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20.63"/>
@@ -402,25 +436,25 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="n">
+      <c r="C2" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="n">
         <v>280</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="3" t="n">
@@ -428,25 +462,25 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="n">
+      <c r="C3" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3" t="n">
         <v>357</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="3" t="n">
@@ -454,25 +488,25 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="3" t="n">
         <v>175</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="3" t="n">
@@ -480,25 +514,25 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="n">
+      <c r="B5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3" t="n">
         <v>316</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="F5" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="3" t="n">
@@ -506,25 +540,25 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1" t="n">
+      <c r="C6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3" t="n">
         <v>335</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="F6" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="3" t="n">
@@ -532,25 +566,25 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="F7" s="1" t="n">
+      <c r="F7" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="3" t="n">
@@ -558,25 +592,25 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D8" s="1" t="n">
+      <c r="C8" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3" t="n">
         <v>270</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="F8" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="3" t="n">
@@ -584,25 +618,25 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="3" t="n">
         <v>453</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="F9" s="1" t="n">
+      <c r="F9" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="3" t="n">
@@ -610,25 +644,25 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D10" s="1" t="n">
+      <c r="C10" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3" t="n">
         <v>360</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="F10" s="1" t="n">
+      <c r="F10" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="3" t="n">
@@ -636,25 +670,25 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="3" t="n">
         <v>181</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="F11" s="1" t="n">
+      <c r="F11" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="3" t="n">
@@ -662,25 +696,25 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="3" t="n">
         <v>443</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="F12" s="1" t="n">
+      <c r="F12" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H12" s="3" t="n">
@@ -688,25 +722,25 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="C13" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D13" s="1" t="n">
+      <c r="C13" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3" t="n">
         <v>340</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="F13" s="1" t="n">
+      <c r="F13" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H13" s="3" t="n">
@@ -714,25 +748,25 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="C14" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D14" s="1" t="n">
+      <c r="C14" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D14" s="3" t="n">
         <v>355</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="F14" s="1" t="n">
+      <c r="F14" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H14" s="3" t="n">
@@ -740,25 +774,25 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C15" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="3" t="n">
         <v>390</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="F15" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H15" s="3" t="n">
@@ -766,25 +800,25 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="1" t="n">
+      <c r="B16" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="C16" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D16" s="1" t="n">
+      <c r="C16" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D16" s="3" t="n">
         <v>372</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="E16" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="F16" s="1" t="n">
+      <c r="F16" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H16" s="3" t="n">
@@ -792,25 +826,25 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="1" t="n">
+      <c r="B17" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="C17" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D17" s="1" t="n">
+      <c r="C17" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D17" s="3" t="n">
         <v>324</v>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="F17" s="1" t="n">
+      <c r="F17" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H17" s="3" t="n">
@@ -818,25 +852,25 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="1" t="n">
+      <c r="B18" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="C18" s="1" t="n">
+      <c r="C18" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="3" t="n">
         <v>140</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="F18" s="1" t="n">
+      <c r="F18" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H18" s="3" t="n">
@@ -844,25 +878,25 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="1" t="n">
+      <c r="B19" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="C19" s="1" t="n">
+      <c r="C19" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="3" t="n">
         <v>491</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="F19" s="1" t="n">
+      <c r="F19" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H19" s="3" t="n">
@@ -870,259 +904,259 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="1" t="n">
+      <c r="B20" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C20" s="1" t="n">
+      <c r="C20" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="D20" s="3" t="n">
         <v>90</v>
       </c>
-      <c r="E20" s="1" t="n">
+      <c r="E20" s="3" t="n">
         <v>30.5</v>
       </c>
-      <c r="F20" s="1" t="n">
+      <c r="F20" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="1" t="n">
+      <c r="H20" s="3" t="n">
         <v>174.905305588994</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="1" t="n">
+      <c r="B21" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C21" s="1" t="n">
+      <c r="C21" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="3" t="n">
         <v>125</v>
       </c>
-      <c r="E21" s="1" t="n">
+      <c r="E21" s="3" t="n">
         <v>30.5</v>
       </c>
-      <c r="F21" s="1" t="n">
+      <c r="F21" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H21" s="1" t="n">
+      <c r="H21" s="3" t="n">
         <v>174.905305588994</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="1" t="n">
+      <c r="B22" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C22" s="1" t="n">
+      <c r="C22" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="1" t="n">
+      <c r="D22" s="3" t="n">
         <v>150</v>
       </c>
-      <c r="E22" s="1" t="n">
+      <c r="E22" s="3" t="n">
         <v>30.5</v>
       </c>
-      <c r="F22" s="1" t="n">
+      <c r="F22" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="1" t="n">
+      <c r="H22" s="3" t="n">
         <v>174.905305588994</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D23" s="1" t="n">
+      <c r="B23" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D23" s="3" t="n">
         <v>355</v>
       </c>
-      <c r="E23" s="1" t="n">
+      <c r="E23" s="3" t="n">
         <v>30.5</v>
       </c>
-      <c r="F23" s="1" t="n">
+      <c r="F23" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="1" t="n">
+      <c r="H23" s="3" t="n">
         <v>174.905305588994</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="1" t="n">
+      <c r="B24" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C24" s="1" t="n">
+      <c r="C24" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D24" s="1" t="n">
+      <c r="D24" s="3" t="n">
         <v>102</v>
       </c>
-      <c r="E24" s="1" t="n">
+      <c r="E24" s="3" t="n">
         <v>30.5</v>
       </c>
-      <c r="F24" s="1" t="n">
+      <c r="F24" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="1" t="n">
+      <c r="H24" s="3" t="n">
         <v>174.905305588994</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="1" t="n">
+      <c r="B25" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="C25" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D25" s="1" t="n">
+      <c r="C25" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D25" s="3" t="n">
         <v>240</v>
       </c>
-      <c r="E25" s="1" t="n">
+      <c r="E25" s="3" t="n">
         <v>30.5</v>
       </c>
-      <c r="F25" s="1" t="n">
+      <c r="F25" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="1" t="n">
+      <c r="H25" s="3" t="n">
         <v>174.905305588994</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="1" t="n">
+      <c r="B26" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C26" s="1" t="n">
+      <c r="C26" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="D26" s="3" t="n">
         <v>137</v>
       </c>
-      <c r="E26" s="1" t="n">
+      <c r="E26" s="3" t="n">
         <v>30.5</v>
       </c>
-      <c r="F26" s="1" t="n">
+      <c r="F26" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H26" s="1" t="n">
+      <c r="H26" s="3" t="n">
         <v>174.905305588994</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="1" t="n">
+      <c r="B27" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C27" s="1" t="n">
+      <c r="C27" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D27" s="1" t="n">
+      <c r="D27" s="3" t="n">
         <v>178</v>
       </c>
-      <c r="E27" s="1" t="n">
+      <c r="E27" s="3" t="n">
         <v>30.5</v>
       </c>
-      <c r="F27" s="1" t="n">
+      <c r="F27" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="1" t="n">
+      <c r="H27" s="3" t="n">
         <v>174.905305588994</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="1" t="n">
+      <c r="B28" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C28" s="1" t="n">
+      <c r="C28" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D28" s="1" t="n">
+      <c r="D28" s="3" t="n">
         <v>113</v>
       </c>
-      <c r="E28" s="1" t="n">
+      <c r="E28" s="3" t="n">
         <v>30.5</v>
       </c>
-      <c r="F28" s="1" t="n">
+      <c r="F28" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H28" s="1" t="n">
+      <c r="H28" s="3" t="n">
         <v>174.905305588994</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="1" t="n">
+      <c r="B29" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C29" s="1" t="n">
+      <c r="C29" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D29" s="1" t="n">
+      <c r="D29" s="3" t="n">
         <v>410</v>
       </c>
-      <c r="E29" s="1" t="n">
+      <c r="E29" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="F29" s="1" t="n">
+      <c r="F29" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H29" s="3" t="n">
@@ -1130,25 +1164,25 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="1" t="n">
+      <c r="B30" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C30" s="1" t="n">
+      <c r="C30" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D30" s="1" t="n">
+      <c r="D30" s="3" t="n">
         <v>420</v>
       </c>
-      <c r="E30" s="1" t="n">
+      <c r="E30" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="F30" s="1" t="n">
+      <c r="F30" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H30" s="3" t="n">
@@ -1156,25 +1190,25 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="1" t="n">
+      <c r="B31" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C31" s="1" t="n">
+      <c r="C31" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D31" s="1" t="n">
+      <c r="D31" s="3" t="n">
         <v>187</v>
       </c>
-      <c r="E31" s="1" t="n">
+      <c r="E31" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="F31" s="1" t="n">
+      <c r="F31" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H31" s="3" t="n">
@@ -1182,25 +1216,25 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C32" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D32" s="1" t="n">
+      <c r="B32" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C32" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D32" s="3" t="n">
         <v>225</v>
       </c>
-      <c r="E32" s="1" t="n">
+      <c r="E32" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="F32" s="1" t="n">
+      <c r="F32" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H32" s="3" t="n">
@@ -1208,25 +1242,25 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="1" t="n">
+      <c r="B33" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C33" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D33" s="1" t="n">
+      <c r="C33" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D33" s="3" t="n">
         <v>326</v>
       </c>
-      <c r="E33" s="1" t="n">
+      <c r="E33" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="F33" s="1" t="n">
+      <c r="F33" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H33" s="3" t="n">
@@ -1234,25 +1268,25 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="1" t="n">
+      <c r="B34" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="C34" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D34" s="1" t="n">
+      <c r="C34" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D34" s="3" t="n">
         <v>360</v>
       </c>
-      <c r="E34" s="1" t="n">
+      <c r="E34" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="F34" s="1" t="n">
+      <c r="F34" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H34" s="3" t="n">
@@ -1260,25 +1294,25 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="1" t="n">
+      <c r="B35" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C35" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D35" s="1" t="n">
+      <c r="C35" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D35" s="3" t="n">
         <v>406</v>
       </c>
-      <c r="E35" s="1" t="n">
+      <c r="E35" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="F35" s="1" t="n">
+      <c r="F35" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H35" s="3" t="n">
@@ -1286,25 +1320,25 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="1" t="n">
+      <c r="B36" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C36" s="1" t="n">
+      <c r="C36" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D36" s="1" t="n">
+      <c r="D36" s="3" t="n">
         <v>114</v>
       </c>
-      <c r="E36" s="1" t="n">
+      <c r="E36" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="F36" s="1" t="n">
+      <c r="F36" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G36" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H36" s="3" t="n">
@@ -1312,25 +1346,25 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="1" t="n">
+      <c r="B37" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C37" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D37" s="1" t="n">
+      <c r="C37" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D37" s="3" t="n">
         <v>356</v>
       </c>
-      <c r="E37" s="1" t="n">
+      <c r="E37" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="F37" s="1" t="n">
+      <c r="F37" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G37" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H37" s="3" t="n">
@@ -1338,25 +1372,25 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="1" t="n">
+      <c r="B38" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="C38" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D38" s="1" t="n">
+      <c r="C38" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D38" s="3" t="n">
         <v>357</v>
       </c>
-      <c r="E38" s="1" t="n">
+      <c r="E38" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="F38" s="1" t="n">
+      <c r="F38" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G38" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H38" s="3" t="n">
@@ -1364,25 +1398,25 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="1" t="n">
+      <c r="B39" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="C39" s="1" t="n">
+      <c r="C39" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D39" s="1" t="n">
+      <c r="D39" s="3" t="n">
         <v>159</v>
       </c>
-      <c r="E39" s="1" t="n">
+      <c r="E39" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="F39" s="1" t="n">
+      <c r="F39" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G39" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H39" s="3" t="n">
@@ -1390,25 +1424,25 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="1" t="n">
+      <c r="B40" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="C40" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D40" s="1" t="n">
+      <c r="C40" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D40" s="3" t="n">
         <v>298</v>
       </c>
-      <c r="E40" s="1" t="n">
+      <c r="E40" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="F40" s="1" t="n">
+      <c r="F40" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="G40" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H40" s="3" t="n">
@@ -1416,25 +1450,25 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="1" t="n">
+      <c r="B41" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="C41" s="1" t="n">
+      <c r="C41" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D41" s="1" t="n">
+      <c r="D41" s="3" t="n">
         <v>129</v>
       </c>
-      <c r="E41" s="1" t="n">
+      <c r="E41" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="F41" s="1" t="n">
+      <c r="F41" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G41" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H41" s="3" t="n">
@@ -1442,25 +1476,25 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="1" t="n">
+      <c r="B42" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="C42" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D42" s="1" t="n">
+      <c r="C42" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D42" s="3" t="n">
         <v>305</v>
       </c>
-      <c r="E42" s="1" t="n">
+      <c r="E42" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="F42" s="1" t="n">
+      <c r="F42" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G42" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H42" s="3" t="n">
@@ -1468,25 +1502,25 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="1" t="n">
+      <c r="B43" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="C43" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D43" s="1" t="n">
+      <c r="C43" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D43" s="3" t="n">
         <v>318</v>
       </c>
-      <c r="E43" s="1" t="n">
+      <c r="E43" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="F43" s="1" t="n">
+      <c r="F43" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G43" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H43" s="3" t="n">
@@ -1494,25 +1528,25 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="1" t="n">
+      <c r="B44" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="C44" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D44" s="1" t="n">
+      <c r="C44" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D44" s="3" t="n">
         <v>326</v>
       </c>
-      <c r="E44" s="1" t="n">
+      <c r="E44" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="F44" s="1" t="n">
+      <c r="F44" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G44" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H44" s="3" t="n">
@@ -1520,25 +1554,25 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B45" s="1" t="n">
+      <c r="B45" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="C45" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D45" s="1" t="n">
+      <c r="C45" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D45" s="3" t="n">
         <v>327</v>
       </c>
-      <c r="E45" s="1" t="n">
+      <c r="E45" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="F45" s="1" t="n">
+      <c r="F45" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="G45" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H45" s="3" t="n">
@@ -1546,25 +1580,25 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="1" t="n">
+      <c r="B46" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="C46" s="1" t="n">
+      <c r="C46" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D46" s="1" t="n">
+      <c r="D46" s="3" t="n">
         <v>453</v>
       </c>
-      <c r="E46" s="1" t="n">
+      <c r="E46" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="F46" s="1" t="n">
+      <c r="F46" s="3" t="n">
         <v>115</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="G46" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H46" s="3" t="n">
@@ -1572,25 +1606,25 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="1" t="n">
+      <c r="B47" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C47" s="1" t="n">
+      <c r="C47" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D47" s="1" t="n">
+      <c r="D47" s="3" t="n">
         <v>468</v>
       </c>
-      <c r="E47" s="1" t="n">
+      <c r="E47" s="3" t="n">
         <v>68.1</v>
       </c>
-      <c r="F47" s="1" t="n">
+      <c r="F47" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="G47" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H47" s="3" t="n">
@@ -1598,25 +1632,25 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="1" t="n">
+      <c r="B48" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C48" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D48" s="1" t="n">
+      <c r="C48" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D48" s="3" t="n">
         <v>266</v>
       </c>
-      <c r="E48" s="1" t="n">
+      <c r="E48" s="3" t="n">
         <v>68.1</v>
       </c>
-      <c r="F48" s="1" t="n">
+      <c r="F48" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="G48" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H48" s="3" t="n">
@@ -1624,25 +1658,25 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="1" t="n">
+      <c r="B49" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C49" s="1" t="n">
+      <c r="C49" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D49" s="1" t="n">
+      <c r="D49" s="3" t="n">
         <v>132</v>
       </c>
-      <c r="E49" s="1" t="n">
+      <c r="E49" s="3" t="n">
         <v>68.1</v>
       </c>
-      <c r="F49" s="1" t="n">
+      <c r="F49" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="G49" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H49" s="3" t="n">
@@ -1650,25 +1684,25 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B50" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C50" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D50" s="1" t="n">
+      <c r="B50" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C50" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D50" s="3" t="n">
         <v>326</v>
       </c>
-      <c r="E50" s="1" t="n">
+      <c r="E50" s="3" t="n">
         <v>68.1</v>
       </c>
-      <c r="F50" s="1" t="n">
+      <c r="F50" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="G50" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H50" s="3" t="n">
@@ -1676,25 +1710,25 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B51" s="1" t="n">
+      <c r="B51" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C51" s="1" t="n">
+      <c r="C51" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D51" s="1" t="n">
+      <c r="D51" s="3" t="n">
         <v>174</v>
       </c>
-      <c r="E51" s="1" t="n">
+      <c r="E51" s="3" t="n">
         <v>68.1</v>
       </c>
-      <c r="F51" s="1" t="n">
+      <c r="F51" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="G51" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H51" s="3" t="n">
@@ -1702,25 +1736,25 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B52" s="1" t="n">
+      <c r="B52" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="C52" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D52" s="1" t="n">
+      <c r="C52" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D52" s="3" t="n">
         <v>263</v>
       </c>
-      <c r="E52" s="1" t="n">
+      <c r="E52" s="3" t="n">
         <v>68.1</v>
       </c>
-      <c r="F52" s="1" t="n">
+      <c r="F52" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="G52" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H52" s="3" t="n">
@@ -1728,25 +1762,25 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="1" t="n">
+      <c r="B53" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C53" s="1" t="n">
+      <c r="C53" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D53" s="1" t="n">
+      <c r="D53" s="3" t="n">
         <v>515</v>
       </c>
-      <c r="E53" s="1" t="n">
+      <c r="E53" s="3" t="n">
         <v>68.1</v>
       </c>
-      <c r="F53" s="1" t="n">
+      <c r="F53" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="G53" s="1" t="s">
+      <c r="G53" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H53" s="3" t="n">
@@ -1754,25 +1788,25 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B54" s="1" t="n">
+      <c r="B54" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C54" s="1" t="n">
+      <c r="C54" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D54" s="1" t="n">
+      <c r="D54" s="3" t="n">
         <v>128</v>
       </c>
-      <c r="E54" s="1" t="n">
+      <c r="E54" s="3" t="n">
         <v>68.1</v>
       </c>
-      <c r="F54" s="1" t="n">
+      <c r="F54" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="G54" s="1" t="s">
+      <c r="G54" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H54" s="3" t="n">
@@ -1780,25 +1814,25 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="1" t="n">
+      <c r="B55" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C55" s="1" t="n">
+      <c r="C55" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D55" s="1" t="n">
+      <c r="D55" s="3" t="n">
         <v>450</v>
       </c>
-      <c r="E55" s="1" t="n">
+      <c r="E55" s="3" t="n">
         <v>68.1</v>
       </c>
-      <c r="F55" s="1" t="n">
+      <c r="F55" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="G55" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H55" s="3" t="n">
@@ -1806,25 +1840,25 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B56" s="1" t="n">
+      <c r="B56" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="C56" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D56" s="1" t="n">
+      <c r="C56" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D56" s="3" t="n">
         <v>269</v>
       </c>
-      <c r="E56" s="1" t="n">
+      <c r="E56" s="3" t="n">
         <v>68.1</v>
       </c>
-      <c r="F56" s="1" t="n">
+      <c r="F56" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="G56" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H56" s="3" t="n">
@@ -1832,25 +1866,25 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B57" s="1" t="n">
+      <c r="B57" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="C57" s="1" t="n">
+      <c r="C57" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D57" s="1" t="n">
+      <c r="D57" s="3" t="n">
         <v>177</v>
       </c>
-      <c r="E57" s="1" t="n">
+      <c r="E57" s="3" t="n">
         <v>68.1</v>
       </c>
-      <c r="F57" s="1" t="n">
+      <c r="F57" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="G57" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H57" s="3" t="n">
@@ -1858,25 +1892,25 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B58" s="1" t="n">
+      <c r="B58" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="C58" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D58" s="1" t="n">
+      <c r="C58" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D58" s="3" t="n">
         <v>289</v>
       </c>
-      <c r="E58" s="1" t="n">
+      <c r="E58" s="3" t="n">
         <v>68.1</v>
       </c>
-      <c r="F58" s="1" t="n">
+      <c r="F58" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="G58" s="1" t="s">
+      <c r="G58" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H58" s="3" t="n">
@@ -1884,25 +1918,25 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="1" t="n">
+      <c r="B59" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="C59" s="1" t="n">
+      <c r="C59" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D59" s="1" t="n">
+      <c r="D59" s="3" t="n">
         <v>187</v>
       </c>
-      <c r="E59" s="1" t="n">
+      <c r="E59" s="3" t="n">
         <v>68.1</v>
       </c>
-      <c r="F59" s="1" t="n">
+      <c r="F59" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="G59" s="1" t="s">
+      <c r="G59" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H59" s="3" t="n">
@@ -1910,25 +1944,25 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B60" s="1" t="n">
+      <c r="B60" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="C60" s="1" t="n">
+      <c r="C60" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D60" s="1" t="n">
+      <c r="D60" s="3" t="n">
         <v>472</v>
       </c>
-      <c r="E60" s="1" t="n">
+      <c r="E60" s="3" t="n">
         <v>68.1</v>
       </c>
-      <c r="F60" s="1" t="n">
+      <c r="F60" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="G60" s="1" t="s">
+      <c r="G60" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H60" s="3" t="n">
@@ -1936,25 +1970,25 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B61" s="1" t="n">
+      <c r="B61" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="C61" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D61" s="1" t="n">
+      <c r="C61" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D61" s="3" t="n">
         <v>288</v>
       </c>
-      <c r="E61" s="1" t="n">
+      <c r="E61" s="3" t="n">
         <v>68.1</v>
       </c>
-      <c r="F61" s="1" t="n">
+      <c r="F61" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="G61" s="1" t="s">
+      <c r="G61" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H61" s="3" t="n">
@@ -1962,25 +1996,25 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B62" s="1" t="n">
+      <c r="B62" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="C62" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D62" s="1" t="n">
+      <c r="C62" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D62" s="3" t="n">
         <v>370</v>
       </c>
-      <c r="E62" s="1" t="n">
+      <c r="E62" s="3" t="n">
         <v>68.1</v>
       </c>
-      <c r="F62" s="1" t="n">
+      <c r="F62" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="G62" s="1" t="s">
+      <c r="G62" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H62" s="3" t="n">
@@ -1988,25 +2022,25 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B63" s="1" t="n">
+      <c r="B63" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="C63" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D63" s="1" t="n">
+      <c r="C63" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D63" s="3" t="n">
         <v>310</v>
       </c>
-      <c r="E63" s="1" t="n">
+      <c r="E63" s="3" t="n">
         <v>68.1</v>
       </c>
-      <c r="F63" s="1" t="n">
+      <c r="F63" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="G63" s="1" t="s">
+      <c r="G63" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H63" s="3" t="n">
@@ -2014,25 +2048,25 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B64" s="1" t="n">
+      <c r="B64" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="C64" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D64" s="1" t="n">
+      <c r="C64" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D64" s="3" t="n">
         <v>287</v>
       </c>
-      <c r="E64" s="1" t="n">
+      <c r="E64" s="3" t="n">
         <v>68.1</v>
       </c>
-      <c r="F64" s="1" t="n">
+      <c r="F64" s="3" t="n">
         <v>117</v>
       </c>
-      <c r="G64" s="1" t="s">
+      <c r="G64" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H64" s="3" t="n">
@@ -2040,147 +2074,1983 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B65" s="1" t="n">
+      <c r="B65" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F65" s="3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G65" s="3" t="n">
+        <v>-41.3241151446753</v>
+      </c>
+      <c r="H65" s="3" t="n">
+        <v>174.77293858836</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B66" s="1" t="n">
+      <c r="B66" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F66" s="3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G66" s="3" t="n">
+        <v>-41.3241151446753</v>
+      </c>
+      <c r="H66" s="3" t="n">
+        <v>174.77293858836</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B67" s="1" t="n">
+      <c r="B67" s="3" t="n">
         <v>3</v>
       </c>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F67" s="3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G67" s="3" t="n">
+        <v>-41.3241151446753</v>
+      </c>
+      <c r="H67" s="3" t="n">
+        <v>174.77293858836</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B68" s="1" t="n">
-        <v>4</v>
+      <c r="B68" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F68" s="3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G68" s="3" t="n">
+        <v>-41.3241151446753</v>
+      </c>
+      <c r="H68" s="3" t="n">
+        <v>174.77293858836</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B69" s="1" t="n">
+      <c r="B69" s="3" t="n">
         <v>5</v>
       </c>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F69" s="3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G69" s="3" t="n">
+        <v>-41.3241151446753</v>
+      </c>
+      <c r="H69" s="3" t="n">
+        <v>174.77293858836</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B70" s="1" t="n">
+      <c r="B70" s="3" t="n">
         <v>6</v>
       </c>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F70" s="3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G70" s="3" t="n">
+        <v>-41.3241151446753</v>
+      </c>
+      <c r="H70" s="3" t="n">
+        <v>174.77293858836</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B71" s="1" t="n">
+      <c r="B71" s="3" t="n">
         <v>7</v>
       </c>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F71" s="3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G71" s="3" t="n">
+        <v>-41.3241151446753</v>
+      </c>
+      <c r="H71" s="3" t="n">
+        <v>174.77293858836</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B72" s="1" t="n">
+      <c r="B72" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F72" s="3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G72" s="3" t="n">
+        <v>-41.3241151446753</v>
+      </c>
+      <c r="H72" s="3" t="n">
+        <v>174.77293858836</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B73" s="1" t="n">
+      <c r="B73" s="3" t="n">
         <v>9</v>
       </c>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F73" s="3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G73" s="3" t="n">
+        <v>-41.3241151446753</v>
+      </c>
+      <c r="H73" s="3" t="n">
+        <v>174.77293858836</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B74" s="1" t="n">
+      <c r="B74" s="3" t="n">
         <v>10</v>
       </c>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F74" s="3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G74" s="3" t="n">
+        <v>-41.3241151446753</v>
+      </c>
+      <c r="H74" s="3" t="n">
+        <v>174.77293858836</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B75" s="1" t="n">
+      <c r="B75" s="3" t="n">
         <v>11</v>
       </c>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F75" s="3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G75" s="3" t="n">
+        <v>-41.3241151446753</v>
+      </c>
+      <c r="H75" s="3" t="n">
+        <v>174.77293858836</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B76" s="1" t="n">
+      <c r="B76" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F76" s="3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G76" s="3" t="n">
+        <v>-41.3241151446753</v>
+      </c>
+      <c r="H76" s="3" t="n">
+        <v>174.77293858836</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B77" s="1" t="n">
+      <c r="B77" s="3" t="n">
         <v>13</v>
       </c>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F77" s="3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G77" s="3" t="n">
+        <v>-41.3241151446753</v>
+      </c>
+      <c r="H77" s="3" t="n">
+        <v>174.77293858836</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B78" s="1" t="n">
+      <c r="B78" s="3" t="n">
         <v>14</v>
       </c>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F78" s="3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G78" s="3" t="n">
+        <v>-41.3241151446753</v>
+      </c>
+      <c r="H78" s="3" t="n">
+        <v>174.77293858836</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B79" s="1" t="n">
+      <c r="B79" s="3" t="n">
         <v>15</v>
       </c>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F79" s="3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G79" s="3" t="n">
+        <v>-41.3241151446753</v>
+      </c>
+      <c r="H79" s="3" t="n">
+        <v>174.77293858836</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B80" s="1" t="n">
+      <c r="B80" s="3" t="n">
         <v>16</v>
       </c>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F80" s="3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G80" s="3" t="n">
+        <v>-41.3241151446753</v>
+      </c>
+      <c r="H80" s="3" t="n">
+        <v>174.77293858836</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B81" s="1" t="n">
+      <c r="B81" s="3" t="n">
         <v>17</v>
       </c>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F81" s="3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G81" s="3" t="n">
+        <v>-41.3241151446753</v>
+      </c>
+      <c r="H81" s="3" t="n">
+        <v>174.77293858836</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B82" s="1" t="n">
+      <c r="B82" s="3" t="n">
         <v>18</v>
+      </c>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="F82" s="3" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G82" s="3" t="n">
+        <v>-41.3241151446753</v>
+      </c>
+      <c r="H82" s="3" t="n">
+        <v>174.77293858836</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B83" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="3" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F83" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="G83" s="3" t="n">
+        <v>-36.8702429389515</v>
+      </c>
+      <c r="H83" s="3" t="n">
+        <v>174.720759412056</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B84" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="3" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F84" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="G84" s="3" t="n">
+        <v>-36.8702429389515</v>
+      </c>
+      <c r="H84" s="3" t="n">
+        <v>174.720759412056</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B85" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="3" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F85" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="G85" s="3" t="n">
+        <v>-36.8702429389515</v>
+      </c>
+      <c r="H85" s="3" t="n">
+        <v>174.720759412056</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B86" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="3" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F86" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="G86" s="3" t="n">
+        <v>-36.8702429389515</v>
+      </c>
+      <c r="H86" s="3" t="n">
+        <v>174.720759412056</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B87" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="3" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F87" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="G87" s="3" t="n">
+        <v>-36.8702429389515</v>
+      </c>
+      <c r="H87" s="3" t="n">
+        <v>174.720759412056</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B88" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="3" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F88" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="G88" s="3" t="n">
+        <v>-36.8702429389515</v>
+      </c>
+      <c r="H88" s="3" t="n">
+        <v>174.720759412056</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B89" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="3" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F89" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="G89" s="3" t="n">
+        <v>-36.8702429389515</v>
+      </c>
+      <c r="H89" s="3" t="n">
+        <v>174.720759412056</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B90" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="3" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F90" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="G90" s="3" t="n">
+        <v>-36.8702429389515</v>
+      </c>
+      <c r="H90" s="3" t="n">
+        <v>174.720759412056</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B91" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="3" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F91" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="G91" s="3" t="n">
+        <v>-36.8702429389515</v>
+      </c>
+      <c r="H91" s="3" t="n">
+        <v>174.720759412056</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B92" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="3" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F92" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="G92" s="3" t="n">
+        <v>-36.8702429389515</v>
+      </c>
+      <c r="H92" s="3" t="n">
+        <v>174.720759412056</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B93" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="3" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F93" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="G93" s="3" t="n">
+        <v>-36.8702429389515</v>
+      </c>
+      <c r="H93" s="3" t="n">
+        <v>174.720759412056</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B94" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="3" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F94" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="G94" s="3" t="n">
+        <v>-36.8702429389515</v>
+      </c>
+      <c r="H94" s="3" t="n">
+        <v>174.720759412056</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B95" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="3" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F95" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="G95" s="3" t="n">
+        <v>-36.8702429389515</v>
+      </c>
+      <c r="H95" s="3" t="n">
+        <v>174.720759412056</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B96" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="3" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F96" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="G96" s="3" t="n">
+        <v>-36.8702429389515</v>
+      </c>
+      <c r="H96" s="3" t="n">
+        <v>174.720759412056</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B97" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="3" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F97" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="G97" s="3" t="n">
+        <v>-36.8702429389515</v>
+      </c>
+      <c r="H97" s="3" t="n">
+        <v>174.720759412056</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B98" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="3" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F98" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="G98" s="3" t="n">
+        <v>-36.8702429389515</v>
+      </c>
+      <c r="H98" s="3" t="n">
+        <v>174.720759412056</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B99" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="3" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F99" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="G99" s="3" t="n">
+        <v>-36.8702429389515</v>
+      </c>
+      <c r="H99" s="3" t="n">
+        <v>174.720759412056</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B100" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="3" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F100" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="G100" s="3" t="n">
+        <v>-36.8702429389515</v>
+      </c>
+      <c r="H100" s="3" t="n">
+        <v>174.720759412056</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B101" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="3" t="n">
+        <v>72.1</v>
+      </c>
+      <c r="F101" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G101" s="3" t="n">
+        <v>-40.370721643039</v>
+      </c>
+      <c r="H101" s="3" t="n">
+        <v>175.63554374477</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B102" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="3" t="n">
+        <v>72.1</v>
+      </c>
+      <c r="F102" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G102" s="3" t="n">
+        <v>-40.370721643039</v>
+      </c>
+      <c r="H102" s="3" t="n">
+        <v>175.63554374477</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B103" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="3" t="n">
+        <v>72.1</v>
+      </c>
+      <c r="F103" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G103" s="3" t="n">
+        <v>-40.370721643039</v>
+      </c>
+      <c r="H103" s="3" t="n">
+        <v>175.63554374477</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B104" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="3" t="n">
+        <v>72.1</v>
+      </c>
+      <c r="F104" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G104" s="3" t="n">
+        <v>-40.370721643039</v>
+      </c>
+      <c r="H104" s="3" t="n">
+        <v>175.63554374477</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B105" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="3" t="n">
+        <v>72.1</v>
+      </c>
+      <c r="F105" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G105" s="3" t="n">
+        <v>-40.370721643039</v>
+      </c>
+      <c r="H105" s="3" t="n">
+        <v>175.63554374477</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B106" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="3" t="n">
+        <v>72.1</v>
+      </c>
+      <c r="F106" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G106" s="3" t="n">
+        <v>-40.370721643039</v>
+      </c>
+      <c r="H106" s="3" t="n">
+        <v>175.63554374477</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B107" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="3" t="n">
+        <v>72.1</v>
+      </c>
+      <c r="F107" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G107" s="3" t="n">
+        <v>-40.370721643039</v>
+      </c>
+      <c r="H107" s="3" t="n">
+        <v>175.63554374477</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B108" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="3" t="n">
+        <v>72.1</v>
+      </c>
+      <c r="F108" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G108" s="3" t="n">
+        <v>-40.370721643039</v>
+      </c>
+      <c r="H108" s="3" t="n">
+        <v>175.63554374477</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B109" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="3" t="n">
+        <v>72.1</v>
+      </c>
+      <c r="F109" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G109" s="3" t="n">
+        <v>-40.370721643039</v>
+      </c>
+      <c r="H109" s="3" t="n">
+        <v>175.63554374477</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B110" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="3" t="n">
+        <v>72.1</v>
+      </c>
+      <c r="F110" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G110" s="3" t="n">
+        <v>-40.370721643039</v>
+      </c>
+      <c r="H110" s="3" t="n">
+        <v>175.63554374477</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B111" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="3" t="n">
+        <v>72.1</v>
+      </c>
+      <c r="F111" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G111" s="3" t="n">
+        <v>-40.370721643039</v>
+      </c>
+      <c r="H111" s="3" t="n">
+        <v>175.63554374477</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B112" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="3" t="n">
+        <v>72.1</v>
+      </c>
+      <c r="F112" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G112" s="3" t="n">
+        <v>-40.370721643039</v>
+      </c>
+      <c r="H112" s="3" t="n">
+        <v>175.63554374477</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B113" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="C113" s="4"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="3" t="n">
+        <v>72.1</v>
+      </c>
+      <c r="F113" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G113" s="3" t="n">
+        <v>-40.370721643039</v>
+      </c>
+      <c r="H113" s="3" t="n">
+        <v>175.63554374477</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B114" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="C114" s="4"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="3" t="n">
+        <v>72.1</v>
+      </c>
+      <c r="F114" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G114" s="3" t="n">
+        <v>-40.370721643039</v>
+      </c>
+      <c r="H114" s="3" t="n">
+        <v>175.63554374477</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B115" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="3" t="n">
+        <v>72.1</v>
+      </c>
+      <c r="F115" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G115" s="3" t="n">
+        <v>-40.370721643039</v>
+      </c>
+      <c r="H115" s="3" t="n">
+        <v>175.63554374477</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B116" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="C116" s="4"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="3" t="n">
+        <v>72.1</v>
+      </c>
+      <c r="F116" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G116" s="3" t="n">
+        <v>-40.370721643039</v>
+      </c>
+      <c r="H116" s="3" t="n">
+        <v>175.63554374477</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B117" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="C117" s="4"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="3" t="n">
+        <v>72.1</v>
+      </c>
+      <c r="F117" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G117" s="3" t="n">
+        <v>-40.370721643039</v>
+      </c>
+      <c r="H117" s="3" t="n">
+        <v>175.63554374477</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B118" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="3" t="n">
+        <v>72.1</v>
+      </c>
+      <c r="F118" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G118" s="3" t="n">
+        <v>-40.370721643039</v>
+      </c>
+      <c r="H118" s="3" t="n">
+        <v>175.63554374477</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B119" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="3" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="F119" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H119" s="3" t="n">
+        <v>175.643946589925</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B120" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C120" s="4"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="3" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="F120" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H120" s="3" t="n">
+        <v>175.643946589925</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B121" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="3" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="F121" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H121" s="3" t="n">
+        <v>175.643946589925</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B122" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C122" s="4"/>
+      <c r="D122" s="4"/>
+      <c r="E122" s="3" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="F122" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H122" s="3" t="n">
+        <v>175.643946589925</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B123" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C123" s="4"/>
+      <c r="D123" s="4"/>
+      <c r="E123" s="3" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="F123" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H123" s="3" t="n">
+        <v>175.643946589925</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B124" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C124" s="4"/>
+      <c r="D124" s="4"/>
+      <c r="E124" s="3" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="F124" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H124" s="3" t="n">
+        <v>175.643946589925</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B125" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C125" s="4"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="3" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="F125" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H125" s="3" t="n">
+        <v>175.643946589925</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B126" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C126" s="4"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="3" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="F126" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H126" s="3" t="n">
+        <v>175.643946589925</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B127" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="C127" s="4"/>
+      <c r="D127" s="4"/>
+      <c r="E127" s="3" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="F127" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G127" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H127" s="3" t="n">
+        <v>175.643946589925</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B128" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="C128" s="4"/>
+      <c r="D128" s="4"/>
+      <c r="E128" s="3" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="F128" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H128" s="3" t="n">
+        <v>175.643946589925</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B129" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="C129" s="4"/>
+      <c r="D129" s="4"/>
+      <c r="E129" s="3" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="F129" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H129" s="3" t="n">
+        <v>175.643946589925</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B130" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C130" s="4"/>
+      <c r="D130" s="4"/>
+      <c r="E130" s="3" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="F130" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H130" s="3" t="n">
+        <v>175.643946589925</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B131" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="C131" s="4"/>
+      <c r="D131" s="4"/>
+      <c r="E131" s="3" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="F131" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G131" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H131" s="3" t="n">
+        <v>175.643946589925</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B132" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="C132" s="4"/>
+      <c r="D132" s="4"/>
+      <c r="E132" s="3" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="F132" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H132" s="3" t="n">
+        <v>175.643946589925</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B133" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C133" s="4"/>
+      <c r="D133" s="4"/>
+      <c r="E133" s="3" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="F133" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G133" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H133" s="3" t="n">
+        <v>175.643946589925</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B134" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="C134" s="4"/>
+      <c r="D134" s="4"/>
+      <c r="E134" s="3" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="F134" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H134" s="3" t="n">
+        <v>175.643946589925</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B135" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="C135" s="4"/>
+      <c r="D135" s="4"/>
+      <c r="E135" s="3" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="F135" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G135" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H135" s="3" t="n">
+        <v>175.643946589925</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B136" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="C136" s="4"/>
+      <c r="D136" s="4"/>
+      <c r="E136" s="3" t="n">
+        <v>69.9</v>
+      </c>
+      <c r="F136" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="G136" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H136" s="3" t="n">
+        <v>175.643946589925</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B137" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C137" s="4"/>
+      <c r="D137" s="4"/>
+      <c r="E137" s="3" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="F137" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="G137" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H137" s="4" t="n">
+        <v>172.714495227238</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B138" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C138" s="4"/>
+      <c r="D138" s="4"/>
+      <c r="E138" s="3" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="F138" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="G138" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H138" s="4" t="n">
+        <v>172.714495227238</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B139" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C139" s="4"/>
+      <c r="D139" s="4"/>
+      <c r="E139" s="3" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="F139" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="G139" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H139" s="4" t="n">
+        <v>172.714495227238</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B140" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C140" s="4"/>
+      <c r="D140" s="4"/>
+      <c r="E140" s="3" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="F140" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H140" s="4" t="n">
+        <v>172.714495227238</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B141" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C141" s="4"/>
+      <c r="D141" s="4"/>
+      <c r="E141" s="3" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="F141" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="G141" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H141" s="4" t="n">
+        <v>172.714495227238</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B142" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C142" s="4"/>
+      <c r="D142" s="4"/>
+      <c r="E142" s="3" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="F142" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="G142" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H142" s="4" t="n">
+        <v>172.714495227238</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B143" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C143" s="4"/>
+      <c r="D143" s="4"/>
+      <c r="E143" s="3" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="F143" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="G143" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H143" s="4" t="n">
+        <v>172.714495227238</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B144" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C144" s="4"/>
+      <c r="D144" s="4"/>
+      <c r="E144" s="3" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="F144" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="G144" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H144" s="4" t="n">
+        <v>172.714495227238</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B145" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="C145" s="4"/>
+      <c r="D145" s="4"/>
+      <c r="E145" s="3" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="F145" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="G145" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H145" s="4" t="n">
+        <v>172.714495227238</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B146" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="C146" s="4"/>
+      <c r="D146" s="4"/>
+      <c r="E146" s="3" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="F146" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="G146" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H146" s="4" t="n">
+        <v>172.714495227238</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B147" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="C147" s="4"/>
+      <c r="D147" s="4"/>
+      <c r="E147" s="3" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="F147" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="G147" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H147" s="4" t="n">
+        <v>172.714495227238</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B148" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C148" s="4"/>
+      <c r="D148" s="4"/>
+      <c r="E148" s="3" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="F148" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="G148" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H148" s="4" t="n">
+        <v>172.714495227238</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B149" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="C149" s="4"/>
+      <c r="D149" s="4"/>
+      <c r="E149" s="3" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="F149" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="G149" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H149" s="4" t="n">
+        <v>172.714495227238</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B150" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="C150" s="4"/>
+      <c r="D150" s="4"/>
+      <c r="E150" s="3" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="F150" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H150" s="4" t="n">
+        <v>172.714495227238</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B151" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C151" s="4"/>
+      <c r="D151" s="4"/>
+      <c r="E151" s="3" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="F151" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="G151" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H151" s="4" t="n">
+        <v>172.714495227238</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B152" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="C152" s="4"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="3" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="F152" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="G152" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H152" s="4" t="n">
+        <v>172.714495227238</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B153" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="C153" s="4"/>
+      <c r="D153" s="4"/>
+      <c r="E153" s="3" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="F153" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="G153" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H153" s="4" t="n">
+        <v>172.714495227238</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B154" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="C154" s="4"/>
+      <c r="D154" s="4"/>
+      <c r="E154" s="3" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="F154" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H154" s="4" t="n">
+        <v>172.714495227238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat/ adding new data
</commit_message>
<xml_diff>
--- a/app/data/Course_Data.xlsx
+++ b/app/data/Course_Data.xlsx
@@ -173,7 +173,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -190,15 +190,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -394,11 +390,11 @@
   <dimension ref="A1:H154"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H122" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
-      <selection pane="bottomRight" activeCell="J67" activeCellId="0" sqref="J67"/>
+      <selection pane="bottomLeft" activeCell="A122" activeCellId="0" sqref="A122"/>
+      <selection pane="bottomRight" activeCell="D155" activeCellId="0" sqref="D155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3658,14 +3654,18 @@
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="6" t="s">
+      <c r="A137" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B137" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C137" s="4"/>
-      <c r="D137" s="4"/>
+      <c r="C137" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D137" s="4" t="n">
+        <v>466</v>
+      </c>
       <c r="E137" s="3" t="n">
         <v>68.7</v>
       </c>
@@ -3680,14 +3680,18 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="6" t="s">
+      <c r="A138" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B138" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C138" s="4"/>
-      <c r="D138" s="4"/>
+      <c r="C138" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D138" s="4" t="n">
+        <v>355</v>
+      </c>
       <c r="E138" s="3" t="n">
         <v>68.7</v>
       </c>
@@ -3702,14 +3706,18 @@
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="6" t="s">
+      <c r="A139" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B139" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C139" s="4"/>
-      <c r="D139" s="4"/>
+      <c r="C139" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D139" s="4" t="n">
+        <v>356</v>
+      </c>
       <c r="E139" s="3" t="n">
         <v>68.7</v>
       </c>
@@ -3724,14 +3732,18 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="6" t="s">
+      <c r="A140" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B140" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C140" s="4"/>
-      <c r="D140" s="4"/>
+      <c r="C140" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D140" s="4" t="n">
+        <v>398</v>
+      </c>
       <c r="E140" s="3" t="n">
         <v>68.7</v>
       </c>
@@ -3746,14 +3758,18 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="6" t="s">
+      <c r="A141" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B141" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C141" s="4"/>
-      <c r="D141" s="4"/>
+      <c r="C141" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D141" s="4" t="n">
+        <v>159</v>
+      </c>
       <c r="E141" s="3" t="n">
         <v>68.7</v>
       </c>
@@ -3768,14 +3784,18 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="6" t="s">
+      <c r="A142" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B142" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="C142" s="4"/>
-      <c r="D142" s="4"/>
+      <c r="C142" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D142" s="4" t="n">
+        <v>375</v>
+      </c>
       <c r="E142" s="3" t="n">
         <v>68.7</v>
       </c>
@@ -3790,14 +3810,18 @@
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="6" t="s">
+      <c r="A143" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B143" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C143" s="4"/>
-      <c r="D143" s="4"/>
+      <c r="C143" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D143" s="4" t="n">
+        <v>440</v>
+      </c>
       <c r="E143" s="3" t="n">
         <v>68.7</v>
       </c>
@@ -3812,14 +3836,18 @@
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="6" t="s">
+      <c r="A144" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B144" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C144" s="4"/>
-      <c r="D144" s="4"/>
+      <c r="C144" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D144" s="4" t="n">
+        <v>133</v>
+      </c>
       <c r="E144" s="3" t="n">
         <v>68.7</v>
       </c>
@@ -3834,14 +3862,18 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="6" t="s">
+      <c r="A145" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B145" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C145" s="4"/>
-      <c r="D145" s="4"/>
+      <c r="C145" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D145" s="4" t="n">
+        <v>295</v>
+      </c>
       <c r="E145" s="3" t="n">
         <v>68.7</v>
       </c>
@@ -3856,14 +3888,18 @@
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="6" t="s">
+      <c r="A146" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B146" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="C146" s="4"/>
-      <c r="D146" s="4"/>
+      <c r="C146" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D146" s="4" t="n">
+        <v>347</v>
+      </c>
       <c r="E146" s="3" t="n">
         <v>68.7</v>
       </c>
@@ -3878,14 +3914,18 @@
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="6" t="s">
+      <c r="A147" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B147" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="C147" s="4"/>
-      <c r="D147" s="4"/>
+      <c r="C147" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D147" s="4" t="n">
+        <v>319</v>
+      </c>
       <c r="E147" s="3" t="n">
         <v>68.7</v>
       </c>
@@ -3900,14 +3940,18 @@
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="6" t="s">
+      <c r="A148" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B148" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="C148" s="4"/>
-      <c r="D148" s="4"/>
+      <c r="C148" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D148" s="4" t="n">
+        <v>180</v>
+      </c>
       <c r="E148" s="3" t="n">
         <v>68.7</v>
       </c>
@@ -3922,14 +3966,18 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="6" t="s">
+      <c r="A149" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B149" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="C149" s="4"/>
-      <c r="D149" s="4"/>
+      <c r="C149" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D149" s="4" t="n">
+        <v>436</v>
+      </c>
       <c r="E149" s="3" t="n">
         <v>68.7</v>
       </c>
@@ -3944,14 +3992,18 @@
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="6" t="s">
+      <c r="A150" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B150" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="C150" s="4"/>
-      <c r="D150" s="4"/>
+      <c r="C150" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D150" s="4" t="n">
+        <v>274</v>
+      </c>
       <c r="E150" s="3" t="n">
         <v>68.7</v>
       </c>
@@ -3966,14 +4018,18 @@
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="6" t="s">
+      <c r="A151" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B151" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="C151" s="4"/>
-      <c r="D151" s="4"/>
+      <c r="C151" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D151" s="4" t="n">
+        <v>388</v>
+      </c>
       <c r="E151" s="3" t="n">
         <v>68.7</v>
       </c>
@@ -3988,14 +4044,18 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="6" t="s">
+      <c r="A152" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B152" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="C152" s="4"/>
-      <c r="D152" s="4"/>
+      <c r="C152" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D152" s="4" t="n">
+        <v>316</v>
+      </c>
       <c r="E152" s="3" t="n">
         <v>68.7</v>
       </c>
@@ -4010,14 +4070,18 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="6" t="s">
+      <c r="A153" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B153" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="C153" s="4"/>
-      <c r="D153" s="4"/>
+      <c r="C153" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D153" s="4" t="n">
+        <v>150</v>
+      </c>
       <c r="E153" s="3" t="n">
         <v>68.7</v>
       </c>
@@ -4032,14 +4096,18 @@
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="6" t="s">
+      <c r="A154" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B154" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="C154" s="4"/>
-      <c r="D154" s="4"/>
+      <c r="C154" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D154" s="4" t="n">
+        <v>465</v>
+      </c>
       <c r="E154" s="3" t="n">
         <v>68.7</v>
       </c>

</xml_diff>

<commit_message>
feat/ added new data
</commit_message>
<xml_diff>
--- a/app/data/Course_Data.xlsx
+++ b/app/data/Course_Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="24">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -90,6 +90,9 @@
   <si>
     <t xml:space="preserve">-43.48113500900837</t>
   </si>
+  <si>
+    <t xml:space="preserve">Kapiti Golf Course</t>
+  </si>
 </sst>
 </file>
 
@@ -98,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +132,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -173,7 +182,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -196,6 +205,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -387,14 +404,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H154"/>
+  <dimension ref="A1:H164"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H122" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H140" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A122" activeCellId="0" sqref="A122"/>
-      <selection pane="bottomRight" activeCell="D155" activeCellId="0" sqref="D155"/>
+      <selection pane="bottomLeft" activeCell="A140" activeCellId="0" sqref="A140"/>
+      <selection pane="bottomRight" activeCell="K149" activeCellId="0" sqref="K149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4121,6 +4138,250 @@
         <v>172.714495227238</v>
       </c>
     </row>
+    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B155" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C155" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D155" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E155" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="F155" s="4" t="n">
+        <v>102</v>
+      </c>
+      <c r="G155" s="4" t="n">
+        <v>-40.9296324816681</v>
+      </c>
+      <c r="H155" s="7" t="n">
+        <v>175.010768880422</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B156" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C156" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D156" s="6" t="n">
+        <v>173</v>
+      </c>
+      <c r="E156" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="F156" s="4" t="n">
+        <v>102</v>
+      </c>
+      <c r="G156" s="4" t="n">
+        <v>-40.9296324816681</v>
+      </c>
+      <c r="H156" s="7" t="n">
+        <v>175.010768880422</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B157" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C157" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D157" s="6" t="n">
+        <v>249</v>
+      </c>
+      <c r="E157" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="F157" s="4" t="n">
+        <v>102</v>
+      </c>
+      <c r="G157" s="4" t="n">
+        <v>-40.9296324816681</v>
+      </c>
+      <c r="H157" s="7" t="n">
+        <v>175.010768880422</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B158" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C158" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D158" s="6" t="n">
+        <v>168</v>
+      </c>
+      <c r="E158" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="F158" s="4" t="n">
+        <v>102</v>
+      </c>
+      <c r="G158" s="4" t="n">
+        <v>-40.9296324816681</v>
+      </c>
+      <c r="H158" s="7" t="n">
+        <v>175.010768880422</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B159" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C159" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D159" s="6" t="n">
+        <v>363</v>
+      </c>
+      <c r="E159" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="F159" s="4" t="n">
+        <v>102</v>
+      </c>
+      <c r="G159" s="4" t="n">
+        <v>-40.9296324816681</v>
+      </c>
+      <c r="H159" s="7" t="n">
+        <v>175.010768880422</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B160" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C160" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D160" s="6" t="n">
+        <v>223</v>
+      </c>
+      <c r="E160" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="F160" s="4" t="n">
+        <v>102</v>
+      </c>
+      <c r="G160" s="4" t="n">
+        <v>-40.9296324816681</v>
+      </c>
+      <c r="H160" s="7" t="n">
+        <v>175.010768880422</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B161" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C161" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D161" s="6" t="n">
+        <v>262</v>
+      </c>
+      <c r="E161" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="F161" s="4" t="n">
+        <v>102</v>
+      </c>
+      <c r="G161" s="4" t="n">
+        <v>-40.9296324816681</v>
+      </c>
+      <c r="H161" s="7" t="n">
+        <v>175.010768880422</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B162" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C162" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D162" s="6" t="n">
+        <v>281</v>
+      </c>
+      <c r="E162" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="F162" s="4" t="n">
+        <v>102</v>
+      </c>
+      <c r="G162" s="4" t="n">
+        <v>-40.9296324816681</v>
+      </c>
+      <c r="H162" s="7" t="n">
+        <v>175.010768880422</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B163" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="C163" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D163" s="6" t="n">
+        <v>343</v>
+      </c>
+      <c r="E163" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="F163" s="4" t="n">
+        <v>102</v>
+      </c>
+      <c r="G163" s="4" t="n">
+        <v>-40.9296324816681</v>
+      </c>
+      <c r="H163" s="7" t="n">
+        <v>175.010768880422</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="4"/>
+      <c r="B164" s="6"/>
+      <c r="C164" s="6"/>
+      <c r="D164" s="6"/>
+      <c r="E164" s="4"/>
+      <c r="F164" s="4"/>
+      <c r="G164" s="4"/>
+      <c r="H164" s="6"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
feat/ fixed a dataloader thing and added more courses
</commit_message>
<xml_diff>
--- a/app/data/Course_Data.xlsx
+++ b/app/data/Course_Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="26">
   <si>
     <t xml:space="preserve">Course</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t xml:space="preserve">Kapiti Golf Course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Levin Golf Course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-40.59456674608564</t>
   </si>
 </sst>
 </file>
@@ -207,11 +213,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -404,14 +410,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H164"/>
+  <dimension ref="A1:H182"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H140" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H146" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A140" activeCellId="0" sqref="A140"/>
-      <selection pane="bottomRight" activeCell="K149" activeCellId="0" sqref="K149"/>
+      <selection pane="bottomLeft" activeCell="A146" activeCellId="0" sqref="A146"/>
+      <selection pane="bottomRight" activeCell="F168" activeCellId="0" sqref="F168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4145,10 +4151,10 @@
       <c r="B155" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C155" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D155" s="6" t="n">
+      <c r="C155" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D155" s="4" t="n">
         <v>269</v>
       </c>
       <c r="E155" s="4" t="n">
@@ -4160,7 +4166,7 @@
       <c r="G155" s="4" t="n">
         <v>-40.9296324816681</v>
       </c>
-      <c r="H155" s="7" t="n">
+      <c r="H155" s="3" t="n">
         <v>175.010768880422</v>
       </c>
     </row>
@@ -4171,10 +4177,10 @@
       <c r="B156" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C156" s="6" t="n">
+      <c r="C156" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D156" s="6" t="n">
+      <c r="D156" s="4" t="n">
         <v>173</v>
       </c>
       <c r="E156" s="4" t="n">
@@ -4186,7 +4192,7 @@
       <c r="G156" s="4" t="n">
         <v>-40.9296324816681</v>
       </c>
-      <c r="H156" s="7" t="n">
+      <c r="H156" s="3" t="n">
         <v>175.010768880422</v>
       </c>
     </row>
@@ -4197,10 +4203,10 @@
       <c r="B157" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C157" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D157" s="6" t="n">
+      <c r="C157" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D157" s="4" t="n">
         <v>249</v>
       </c>
       <c r="E157" s="4" t="n">
@@ -4212,7 +4218,7 @@
       <c r="G157" s="4" t="n">
         <v>-40.9296324816681</v>
       </c>
-      <c r="H157" s="7" t="n">
+      <c r="H157" s="3" t="n">
         <v>175.010768880422</v>
       </c>
     </row>
@@ -4223,10 +4229,10 @@
       <c r="B158" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C158" s="6" t="n">
+      <c r="C158" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D158" s="6" t="n">
+      <c r="D158" s="4" t="n">
         <v>168</v>
       </c>
       <c r="E158" s="4" t="n">
@@ -4238,7 +4244,7 @@
       <c r="G158" s="4" t="n">
         <v>-40.9296324816681</v>
       </c>
-      <c r="H158" s="7" t="n">
+      <c r="H158" s="3" t="n">
         <v>175.010768880422</v>
       </c>
     </row>
@@ -4249,10 +4255,10 @@
       <c r="B159" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C159" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D159" s="6" t="n">
+      <c r="C159" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D159" s="4" t="n">
         <v>363</v>
       </c>
       <c r="E159" s="4" t="n">
@@ -4264,7 +4270,7 @@
       <c r="G159" s="4" t="n">
         <v>-40.9296324816681</v>
       </c>
-      <c r="H159" s="7" t="n">
+      <c r="H159" s="3" t="n">
         <v>175.010768880422</v>
       </c>
     </row>
@@ -4275,10 +4281,10 @@
       <c r="B160" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="C160" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D160" s="6" t="n">
+      <c r="C160" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D160" s="4" t="n">
         <v>223</v>
       </c>
       <c r="E160" s="4" t="n">
@@ -4290,7 +4296,7 @@
       <c r="G160" s="4" t="n">
         <v>-40.9296324816681</v>
       </c>
-      <c r="H160" s="7" t="n">
+      <c r="H160" s="3" t="n">
         <v>175.010768880422</v>
       </c>
     </row>
@@ -4301,10 +4307,10 @@
       <c r="B161" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C161" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D161" s="6" t="n">
+      <c r="C161" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D161" s="4" t="n">
         <v>262</v>
       </c>
       <c r="E161" s="4" t="n">
@@ -4316,7 +4322,7 @@
       <c r="G161" s="4" t="n">
         <v>-40.9296324816681</v>
       </c>
-      <c r="H161" s="7" t="n">
+      <c r="H161" s="3" t="n">
         <v>175.010768880422</v>
       </c>
     </row>
@@ -4327,10 +4333,10 @@
       <c r="B162" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C162" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D162" s="6" t="n">
+      <c r="C162" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D162" s="4" t="n">
         <v>281</v>
       </c>
       <c r="E162" s="4" t="n">
@@ -4342,7 +4348,7 @@
       <c r="G162" s="4" t="n">
         <v>-40.9296324816681</v>
       </c>
-      <c r="H162" s="7" t="n">
+      <c r="H162" s="3" t="n">
         <v>175.010768880422</v>
       </c>
     </row>
@@ -4353,10 +4359,10 @@
       <c r="B163" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C163" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D163" s="6" t="n">
+      <c r="C163" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D163" s="4" t="n">
         <v>343</v>
       </c>
       <c r="E163" s="4" t="n">
@@ -4368,19 +4374,444 @@
       <c r="G163" s="4" t="n">
         <v>-40.9296324816681</v>
       </c>
-      <c r="H163" s="7" t="n">
+      <c r="H163" s="3" t="n">
         <v>175.010768880422</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="4"/>
-      <c r="B164" s="6"/>
-      <c r="C164" s="6"/>
-      <c r="D164" s="6"/>
-      <c r="E164" s="4"/>
-      <c r="F164" s="4"/>
-      <c r="G164" s="4"/>
-      <c r="H164" s="6"/>
+      <c r="A164" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B164" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C164" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D164" s="4"/>
+      <c r="E164" s="4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F164" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="G164" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H164" s="6" t="n">
+        <v>175.234684182805</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B165" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C165" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D165" s="7"/>
+      <c r="E165" s="4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F165" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="G165" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H165" s="6" t="n">
+        <v>175.234684182805</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B166" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C166" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D166" s="7"/>
+      <c r="E166" s="4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F166" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="G166" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H166" s="6" t="n">
+        <v>175.234684182805</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B167" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C167" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D167" s="7"/>
+      <c r="E167" s="4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F167" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="G167" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H167" s="6" t="n">
+        <v>175.234684182805</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B168" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C168" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D168" s="7"/>
+      <c r="E168" s="4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F168" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="G168" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H168" s="6" t="n">
+        <v>175.234684182805</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B169" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="C169" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D169" s="7"/>
+      <c r="E169" s="4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F169" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="G169" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H169" s="6" t="n">
+        <v>175.234684182805</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B170" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="C170" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D170" s="7"/>
+      <c r="E170" s="4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F170" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="G170" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H170" s="6" t="n">
+        <v>175.234684182805</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B171" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C171" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D171" s="7"/>
+      <c r="E171" s="4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F171" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="G171" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H171" s="6" t="n">
+        <v>175.234684182805</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B172" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C172" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D172" s="7"/>
+      <c r="E172" s="4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F172" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="G172" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H172" s="6" t="n">
+        <v>175.234684182805</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B173" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="C173" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D173" s="7"/>
+      <c r="E173" s="4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F173" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="G173" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H173" s="6" t="n">
+        <v>175.234684182805</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B174" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="C174" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D174" s="7"/>
+      <c r="E174" s="4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F174" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="G174" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H174" s="6" t="n">
+        <v>175.234684182805</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B175" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="C175" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D175" s="7"/>
+      <c r="E175" s="4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F175" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="G175" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H175" s="6" t="n">
+        <v>175.234684182805</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B176" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="C176" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D176" s="7"/>
+      <c r="E176" s="4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F176" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="G176" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H176" s="6" t="n">
+        <v>175.234684182805</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B177" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="C177" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D177" s="7"/>
+      <c r="E177" s="4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F177" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="G177" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H177" s="6" t="n">
+        <v>175.234684182805</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B178" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="C178" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D178" s="7"/>
+      <c r="E178" s="4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F178" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="G178" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H178" s="6" t="n">
+        <v>175.234684182805</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B179" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="C179" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D179" s="7"/>
+      <c r="E179" s="4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F179" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="G179" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H179" s="6" t="n">
+        <v>175.234684182805</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B180" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="C180" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D180" s="7"/>
+      <c r="E180" s="4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F180" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="G180" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H180" s="6" t="n">
+        <v>175.234684182805</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B181" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="C181" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D181" s="7"/>
+      <c r="E181" s="4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F181" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="G181" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H181" s="6" t="n">
+        <v>175.234684182805</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F182" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>